<commit_message>
Corrections pour les rapports hebdo et annuel
</commit_message>
<xml_diff>
--- a/comptages/report/template.xlsx
+++ b/comptages/report/template.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="210">
   <si>
     <t>Data of the count</t>
   </si>
@@ -592,9 +592,6 @@
     <t>LZ(9)+SZ(10)</t>
   </si>
   <si>
-    <t>W+AH (4)+LIE+AH(6)</t>
-  </si>
-  <si>
     <t>N2 jour</t>
   </si>
   <si>
@@ -687,6 +684,21 @@
   <si>
     <t>%PL</t>
   </si>
+  <si>
+    <t>PW+AH (4)+LIE+AH(6)</t>
+  </si>
+  <si>
+    <t>% PL</t>
+  </si>
+  <si>
+    <t>% VL</t>
+  </si>
+  <si>
+    <t>LZ SZ (19) : Train routier et véhicule lourd articulé</t>
+  </si>
+  <si>
+    <t>Véhicules lourds : CAR (1) + LW (8) + LZ SZ (19)</t>
+  </si>
 </sst>
 </file>
 
@@ -700,7 +712,7 @@
     <numFmt numFmtId="168" formatCode="0.0"/>
     <numFmt numFmtId="169" formatCode="0.00%&quot;       &quot;"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -827,6 +839,11 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1969,7 +1986,7 @@
     <xf numFmtId="0" fontId="19" fillId="16" borderId="81" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="523">
+  <cellXfs count="532">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -3130,7 +3147,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="15" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3187,6 +3203,19 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="76" xfId="6" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="16" borderId="81" xfId="5" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="20" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="17" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="16" borderId="81" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3300,6 +3329,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -4225,7 +4257,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4311,7 +4342,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4360,7 +4390,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5554,7 +5583,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8431,7 +8459,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11315,7 +11342,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12653,8 +12679,8 @@
       <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>965880</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3855</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
@@ -12683,8 +12709,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>965880</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3855</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>160560</xdr:rowOff>
     </xdr:to>
@@ -12719,7 +12745,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>674640</xdr:colOff>
+      <xdr:colOff>636540</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
@@ -12749,7 +12775,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>674640</xdr:colOff>
+      <xdr:colOff>636540</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
@@ -13209,7 +13235,7 @@
   </sheetPr>
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13322,24 +13348,24 @@
       <c r="L10" s="67"/>
     </row>
     <row r="11" spans="1:14" s="5" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="486" t="str">
+      <c r="B11" s="494" t="str">
         <f>"Distrubution des classes SWISS10 par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)"</f>
         <v>Distrubution des classes SWISS10 par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)</v>
       </c>
-      <c r="C11" s="486"/>
-      <c r="D11" s="486"/>
-      <c r="E11" s="486"/>
-      <c r="F11" s="486"/>
-      <c r="G11" s="486"/>
-      <c r="H11" s="486"/>
-      <c r="I11" s="486"/>
-      <c r="J11" s="486"/>
-      <c r="K11" s="486"/>
+      <c r="C11" s="494"/>
+      <c r="D11" s="494"/>
+      <c r="E11" s="494"/>
+      <c r="F11" s="494"/>
+      <c r="G11" s="494"/>
+      <c r="H11" s="494"/>
+      <c r="I11" s="494"/>
+      <c r="J11" s="494"/>
+      <c r="K11" s="494"/>
       <c r="L11" s="305"/>
       <c r="M11" s="234" t="s">
         <v>108</v>
       </c>
-      <c r="N11" s="516" t="s">
+      <c r="N11" s="524" t="s">
         <v>111</v>
       </c>
     </row>
@@ -13381,7 +13407,7 @@
       <c r="M12" s="238" t="s">
         <v>101</v>
       </c>
-      <c r="N12" s="516"/>
+      <c r="N12" s="524"/>
     </row>
     <row r="13" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="239" t="s">
@@ -14842,12 +14868,23 @@
       </c>
     </row>
     <row r="40" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="11"/>
-      <c r="C40" s="10" t="e">
+      <c r="B40" s="484" t="s">
+        <v>207</v>
+      </c>
+      <c r="C40" s="485" t="e">
         <f>SUM(C37:H37)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K40" s="10" t="e">
+      <c r="D40" s="486"/>
+      <c r="E40" s="486"/>
+      <c r="F40" s="486"/>
+      <c r="G40" s="486"/>
+      <c r="H40" s="486"/>
+      <c r="I40" s="486"/>
+      <c r="J40" s="487" t="s">
+        <v>206</v>
+      </c>
+      <c r="K40" s="485" t="e">
         <f>SUM(B37,I37:K37)</f>
         <v>#DIV/0!</v>
       </c>
@@ -14866,24 +14903,24 @@
     </row>
     <row r="43" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5"/>
-      <c r="B43" s="486" t="str">
+      <c r="B43" s="494" t="str">
         <f>B11</f>
         <v>Distrubution des classes SWISS10 par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)</v>
       </c>
-      <c r="C43" s="486"/>
-      <c r="D43" s="486"/>
-      <c r="E43" s="486"/>
-      <c r="F43" s="486"/>
-      <c r="G43" s="486"/>
-      <c r="H43" s="486"/>
-      <c r="I43" s="486"/>
-      <c r="J43" s="486"/>
-      <c r="K43" s="486"/>
+      <c r="C43" s="494"/>
+      <c r="D43" s="494"/>
+      <c r="E43" s="494"/>
+      <c r="F43" s="494"/>
+      <c r="G43" s="494"/>
+      <c r="H43" s="494"/>
+      <c r="I43" s="494"/>
+      <c r="J43" s="494"/>
+      <c r="K43" s="494"/>
       <c r="L43" s="305"/>
       <c r="M43" s="234" t="s">
         <v>108</v>
       </c>
-      <c r="N43" s="516" t="str">
+      <c r="N43" s="524" t="str">
         <f>N11</f>
         <v>Part du TJM</v>
       </c>
@@ -14936,7 +14973,7 @@
       <c r="M44" s="238" t="s">
         <v>101</v>
       </c>
-      <c r="N44" s="516"/>
+      <c r="N44" s="524"/>
     </row>
     <row r="45" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="239" t="s">
@@ -16397,11 +16434,23 @@
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C72" s="10" t="e">
+      <c r="B72" s="484" t="s">
+        <v>207</v>
+      </c>
+      <c r="C72" s="485" t="e">
         <f>SUM(C69:H69)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K72" s="10" t="e">
+      <c r="D72" s="486"/>
+      <c r="E72" s="486"/>
+      <c r="F72" s="486"/>
+      <c r="G72" s="486"/>
+      <c r="H72" s="486"/>
+      <c r="I72" s="486"/>
+      <c r="J72" s="487" t="s">
+        <v>206</v>
+      </c>
+      <c r="K72" s="485" t="e">
         <f>SUM(B69,I69:K69)</f>
         <v>#DIV/0!</v>
       </c>
@@ -16512,10 +16561,10 @@
       <c r="G78" s="67"/>
       <c r="H78" s="67"/>
       <c r="I78" s="67"/>
-      <c r="J78" s="67" t="s">
+      <c r="J78" s="531" t="s">
         <v>164</v>
       </c>
-      <c r="K78" s="349" t="e">
+      <c r="K78" s="491" t="e">
         <f>SUM(B45:B68,B13:B36,I13:K36,I45:K68)/SUM(B45:K68,B13:K36)</f>
         <v>#DIV/0!</v>
       </c>
@@ -16707,17 +16756,17 @@
     </row>
     <row r="11" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L11" s="302"/>
-      <c r="M11" s="515" t="s">
+      <c r="M11" s="523" t="s">
         <v>98</v>
       </c>
-      <c r="N11" s="516" t="s">
+      <c r="N11" s="524" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L12" s="303"/>
-      <c r="M12" s="515"/>
-      <c r="N12" s="516"/>
+      <c r="M12" s="523"/>
+      <c r="N12" s="524"/>
     </row>
     <row r="13" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L13" s="248"/>
@@ -17171,18 +17220,18 @@
     <row r="45" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L46" s="302"/>
-      <c r="M46" s="515" t="s">
+      <c r="M46" s="523" t="s">
         <v>98</v>
       </c>
-      <c r="N46" s="516" t="str">
+      <c r="N46" s="524" t="str">
         <f>N11</f>
         <v>Part du TJM</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L47" s="303"/>
-      <c r="M47" s="515"/>
-      <c r="N47" s="516"/>
+      <c r="M47" s="523"/>
+      <c r="N47" s="524"/>
     </row>
     <row r="48" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L48" s="248"/>
@@ -17752,7 +17801,7 @@
       <c r="A6" s="400"/>
       <c r="C6" s="404"/>
       <c r="E6" s="401" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I6" s="397"/>
     </row>
@@ -17788,20 +17837,20 @@
       <c r="H10" s="409"/>
     </row>
     <row r="11" spans="1:10" s="411" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="517" t="str">
-        <f>"Distrubution des classes SWISS7 par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)"</f>
-        <v>Distrubution des classes SWISS7 par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)</v>
-      </c>
-      <c r="C11" s="517"/>
-      <c r="D11" s="517"/>
-      <c r="E11" s="517"/>
-      <c r="F11" s="517"/>
-      <c r="G11" s="517"/>
+      <c r="B11" s="525" t="str">
+        <f>"Distrubution des classes EUR6 par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)"</f>
+        <v>Distrubution des classes EUR6 par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)</v>
+      </c>
+      <c r="C11" s="525"/>
+      <c r="D11" s="525"/>
+      <c r="E11" s="525"/>
+      <c r="F11" s="525"/>
+      <c r="G11" s="525"/>
       <c r="H11" s="412"/>
       <c r="I11" s="413" t="s">
         <v>108</v>
       </c>
-      <c r="J11" s="518" t="s">
+      <c r="J11" s="526" t="s">
         <v>111</v>
       </c>
     </row>
@@ -17831,7 +17880,7 @@
       <c r="I12" s="418" t="s">
         <v>101</v>
       </c>
-      <c r="J12" s="518"/>
+      <c r="J12" s="526"/>
     </row>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="419" t="s">
@@ -18835,9 +18884,20 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="397"/>
-      <c r="C40" s="452" t="e">
+      <c r="B40" s="487" t="s">
+        <v>207</v>
+      </c>
+      <c r="C40" s="488" t="e">
         <f>SUM(C37:E37)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D40" s="489"/>
+      <c r="E40" s="489"/>
+      <c r="F40" s="487" t="s">
+        <v>206</v>
+      </c>
+      <c r="G40" s="490" t="e">
+        <f>SUM(B37,F37:G37)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J40" s="452"/>
@@ -18856,21 +18916,21 @@
     </row>
     <row r="43" spans="1:10" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="411"/>
-      <c r="B43" s="517" t="str">
+      <c r="B43" s="525" t="str">
         <f>B11</f>
-        <v>Distrubution des classes SWISS7 par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)</v>
-      </c>
-      <c r="C43" s="517"/>
-      <c r="D43" s="517"/>
-      <c r="E43" s="517"/>
-      <c r="F43" s="517"/>
-      <c r="G43" s="517"/>
+        <v>Distrubution des classes EUR6 par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)</v>
+      </c>
+      <c r="C43" s="525"/>
+      <c r="D43" s="525"/>
+      <c r="E43" s="525"/>
+      <c r="F43" s="525"/>
+      <c r="G43" s="525"/>
       <c r="H43" s="412"/>
       <c r="I43" s="413" t="str">
         <f>I11</f>
         <v>THM</v>
       </c>
-      <c r="J43" s="518" t="str">
+      <c r="J43" s="526" t="str">
         <f>J11</f>
         <v>Part du TJM</v>
       </c>
@@ -18907,7 +18967,7 @@
       <c r="I44" s="418" t="s">
         <v>101</v>
       </c>
-      <c r="J44" s="518"/>
+      <c r="J44" s="526"/>
     </row>
     <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="419" t="s">
@@ -19911,7 +19971,22 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C72" s="452"/>
+      <c r="B72" s="487" t="s">
+        <v>207</v>
+      </c>
+      <c r="C72" s="488" t="e">
+        <f>SUM(C69:E69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D72" s="489"/>
+      <c r="E72" s="489"/>
+      <c r="F72" s="487" t="s">
+        <v>206</v>
+      </c>
+      <c r="G72" s="490" t="e">
+        <f>SUM(B69,F69:G69)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="73" spans="1:11" s="455" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="453" t="s">
@@ -19944,7 +20019,7 @@
       <c r="E74" s="453"/>
       <c r="F74" s="453"/>
       <c r="G74" s="453" t="s">
-        <v>126</v>
+        <v>208</v>
       </c>
       <c r="H74" s="409"/>
       <c r="I74" s="409"/>
@@ -19958,9 +20033,7 @@
       <c r="D75" s="453"/>
       <c r="E75" s="453"/>
       <c r="F75" s="453"/>
-      <c r="G75" s="453" t="s">
-        <v>127</v>
-      </c>
+      <c r="G75" s="453"/>
       <c r="H75" s="409"/>
       <c r="I75" s="409"/>
       <c r="J75" s="454"/>
@@ -19974,13 +20047,13 @@
       <c r="C76" s="457"/>
       <c r="D76" s="457"/>
       <c r="E76" s="457"/>
-      <c r="F76" s="519" t="s">
-        <v>129</v>
-      </c>
-      <c r="G76" s="519"/>
-      <c r="H76" s="519"/>
-      <c r="I76" s="519"/>
-      <c r="J76" s="519"/>
+      <c r="F76" s="527" t="s">
+        <v>209</v>
+      </c>
+      <c r="G76" s="527"/>
+      <c r="H76" s="527"/>
+      <c r="I76" s="527"/>
+      <c r="J76" s="527"/>
       <c r="K76" s="456"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -20000,8 +20073,13 @@
       <c r="A78" s="409"/>
       <c r="D78" s="409"/>
       <c r="E78" s="409"/>
-      <c r="F78" s="409"/>
-      <c r="G78" s="458"/>
+      <c r="F78" s="531" t="s">
+        <v>164</v>
+      </c>
+      <c r="G78" s="491" t="e">
+        <f>SUM(B13:B36,B45:B68,F13:G36,F45:G68)/SUM(B13:G36,B45:G68)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="H78" s="409"/>
       <c r="I78" s="409"/>
       <c r="J78" s="454"/>
@@ -20161,7 +20239,7 @@
       <c r="A6" s="400"/>
       <c r="C6" s="404"/>
       <c r="E6" s="401" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I6" s="397"/>
     </row>
@@ -20193,290 +20271,290 @@
       </c>
     </row>
     <row r="10" spans="1:10" s="411" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="459"/>
-      <c r="J10" s="459"/>
+      <c r="B10" s="458"/>
+      <c r="J10" s="458"/>
     </row>
     <row r="11" spans="1:10" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H11" s="460"/>
-      <c r="I11" s="520" t="s">
+      <c r="H11" s="459"/>
+      <c r="I11" s="528" t="s">
         <v>98</v>
       </c>
-      <c r="J11" s="521" t="s">
+      <c r="J11" s="529" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H12" s="461"/>
-      <c r="I12" s="520"/>
-      <c r="J12" s="521"/>
+      <c r="H12" s="460"/>
+      <c r="I12" s="528"/>
+      <c r="J12" s="529"/>
     </row>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H13" s="461"/>
-      <c r="I13" s="462" t="s">
+      <c r="H13" s="460"/>
+      <c r="I13" s="461" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="463" t="e">
+      <c r="J13" s="462" t="e">
         <f>EUR6_H!J13</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H14" s="461"/>
-      <c r="I14" s="464" t="s">
+      <c r="H14" s="460"/>
+      <c r="I14" s="463" t="s">
         <v>27</v>
       </c>
-      <c r="J14" s="465" t="e">
+      <c r="J14" s="464" t="e">
         <f>EUR6_H!J14</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H15" s="461"/>
-      <c r="I15" s="464" t="s">
+      <c r="H15" s="460"/>
+      <c r="I15" s="463" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="465" t="e">
+      <c r="J15" s="464" t="e">
         <f>EUR6_H!J15</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H16" s="461"/>
-      <c r="I16" s="464" t="s">
+      <c r="H16" s="460"/>
+      <c r="I16" s="463" t="s">
         <v>29</v>
       </c>
-      <c r="J16" s="465" t="e">
+      <c r="J16" s="464" t="e">
         <f>EUR6_H!J16</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H17" s="461"/>
-      <c r="I17" s="464" t="s">
+      <c r="H17" s="460"/>
+      <c r="I17" s="463" t="s">
         <v>30</v>
       </c>
-      <c r="J17" s="465" t="e">
+      <c r="J17" s="464" t="e">
         <f>EUR6_H!J17</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H18" s="461"/>
-      <c r="I18" s="464" t="s">
+      <c r="H18" s="460"/>
+      <c r="I18" s="463" t="s">
         <v>31</v>
       </c>
-      <c r="J18" s="465" t="e">
+      <c r="J18" s="464" t="e">
         <f>EUR6_H!J18</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H19" s="461"/>
-      <c r="I19" s="464" t="s">
+      <c r="H19" s="460"/>
+      <c r="I19" s="463" t="s">
         <v>32</v>
       </c>
-      <c r="J19" s="465" t="e">
+      <c r="J19" s="464" t="e">
         <f>EUR6_H!J19</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H20" s="461"/>
+      <c r="H20" s="460"/>
       <c r="I20" s="435" t="s">
         <v>33</v>
       </c>
-      <c r="J20" s="466" t="e">
+      <c r="J20" s="465" t="e">
         <f>EUR6_H!J20</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H21" s="461"/>
-      <c r="I21" s="464" t="s">
+      <c r="H21" s="460"/>
+      <c r="I21" s="463" t="s">
         <v>34</v>
       </c>
-      <c r="J21" s="465" t="e">
+      <c r="J21" s="464" t="e">
         <f>EUR6_H!J21</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="22" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H22" s="461"/>
-      <c r="I22" s="464" t="s">
+      <c r="H22" s="460"/>
+      <c r="I22" s="463" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="465" t="e">
+      <c r="J22" s="464" t="e">
         <f>EUR6_H!J22</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="23" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H23" s="461"/>
-      <c r="I23" s="464" t="s">
+      <c r="H23" s="460"/>
+      <c r="I23" s="463" t="s">
         <v>36</v>
       </c>
-      <c r="J23" s="465" t="e">
+      <c r="J23" s="464" t="e">
         <f>EUR6_H!J23</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="24" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H24" s="461"/>
-      <c r="I24" s="464" t="s">
+      <c r="H24" s="460"/>
+      <c r="I24" s="463" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="465" t="e">
+      <c r="J24" s="464" t="e">
         <f>EUR6_H!J24</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="25" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H25" s="461"/>
-      <c r="I25" s="467" t="s">
+      <c r="H25" s="460"/>
+      <c r="I25" s="466" t="s">
         <v>38</v>
       </c>
-      <c r="J25" s="465" t="e">
+      <c r="J25" s="464" t="e">
         <f>EUR6_H!J25</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="26" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H26" s="461"/>
-      <c r="I26" s="464" t="s">
+      <c r="H26" s="460"/>
+      <c r="I26" s="463" t="s">
         <v>39</v>
       </c>
-      <c r="J26" s="465" t="e">
+      <c r="J26" s="464" t="e">
         <f>EUR6_H!J26</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H27" s="461"/>
-      <c r="I27" s="464" t="s">
+      <c r="H27" s="460"/>
+      <c r="I27" s="463" t="s">
         <v>40</v>
       </c>
-      <c r="J27" s="465" t="e">
+      <c r="J27" s="464" t="e">
         <f>EUR6_H!J27</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="28" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H28" s="461"/>
-      <c r="I28" s="464" t="s">
+      <c r="H28" s="460"/>
+      <c r="I28" s="463" t="s">
         <v>41</v>
       </c>
-      <c r="J28" s="465" t="e">
+      <c r="J28" s="464" t="e">
         <f>EUR6_H!J28</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H29" s="461"/>
-      <c r="I29" s="464" t="s">
+      <c r="H29" s="460"/>
+      <c r="I29" s="463" t="s">
         <v>42</v>
       </c>
-      <c r="J29" s="465" t="e">
+      <c r="J29" s="464" t="e">
         <f>EUR6_H!J29</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="30" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H30" s="461"/>
+      <c r="H30" s="460"/>
       <c r="I30" s="435" t="s">
         <v>43</v>
       </c>
-      <c r="J30" s="466" t="e">
+      <c r="J30" s="465" t="e">
         <f>EUR6_H!J30</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="31" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H31" s="461"/>
-      <c r="I31" s="464" t="s">
+      <c r="H31" s="460"/>
+      <c r="I31" s="463" t="s">
         <v>44</v>
       </c>
-      <c r="J31" s="465" t="e">
+      <c r="J31" s="464" t="e">
         <f>EUR6_H!J31</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H32" s="461"/>
-      <c r="I32" s="464" t="s">
+      <c r="H32" s="460"/>
+      <c r="I32" s="463" t="s">
         <v>45</v>
       </c>
-      <c r="J32" s="465" t="e">
+      <c r="J32" s="464" t="e">
         <f>EUR6_H!J32</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H33" s="461"/>
-      <c r="I33" s="464" t="s">
+      <c r="H33" s="460"/>
+      <c r="I33" s="463" t="s">
         <v>46</v>
       </c>
-      <c r="J33" s="465" t="e">
+      <c r="J33" s="464" t="e">
         <f>EUR6_H!J33</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H34" s="461"/>
-      <c r="I34" s="464" t="s">
+      <c r="H34" s="460"/>
+      <c r="I34" s="463" t="s">
         <v>47</v>
       </c>
-      <c r="J34" s="465" t="e">
+      <c r="J34" s="464" t="e">
         <f>EUR6_H!J34</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H35" s="461"/>
-      <c r="I35" s="464" t="s">
+      <c r="H35" s="460"/>
+      <c r="I35" s="463" t="s">
         <v>48</v>
       </c>
-      <c r="J35" s="465" t="e">
+      <c r="J35" s="464" t="e">
         <f>EUR6_H!J35</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H36" s="468"/>
+      <c r="H36" s="467"/>
       <c r="I36" s="418" t="s">
         <v>49</v>
       </c>
-      <c r="J36" s="469" t="e">
+      <c r="J36" s="468" t="e">
         <f>EUR6_H!J36</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H37" s="409"/>
-      <c r="I37" s="470"/>
-      <c r="J37" s="471"/>
+      <c r="I37" s="469"/>
+      <c r="J37" s="470"/>
     </row>
     <row r="38" spans="1:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="472" t="str">
+      <c r="B38" s="471" t="str">
         <f>EUR6_H!B12</f>
         <v>CAR (1)</v>
       </c>
-      <c r="C38" s="473" t="str">
+      <c r="C38" s="472" t="str">
         <f>EUR6_H!C12</f>
         <v>MR (2)</v>
       </c>
-      <c r="D38" s="474" t="str">
+      <c r="D38" s="473" t="str">
         <f>EUR6_H!D12</f>
         <v>PW (11)</v>
       </c>
-      <c r="E38" s="475" t="str">
+      <c r="E38" s="474" t="str">
         <f>EUR6_H!E12</f>
         <v>LIE (12)</v>
       </c>
-      <c r="F38" s="476" t="str">
+      <c r="F38" s="475" t="str">
         <f>EUR6_H!F12</f>
         <v>LW (8)</v>
       </c>
-      <c r="G38" s="477" t="str">
+      <c r="G38" s="476" t="str">
         <f>EUR6_H!G12</f>
         <v>LZ (9)</v>
       </c>
@@ -20509,9 +20587,9 @@
         <f>EUR6_H!G37</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H39" s="478"/>
+      <c r="H39" s="477"/>
       <c r="I39" s="455"/>
-      <c r="J39" s="479" t="e">
+      <c r="J39" s="478" t="e">
         <f>EUR6_H!J37</f>
         <v>#DIV/0!</v>
       </c>
@@ -20544,9 +20622,9 @@
         <f>EUR6_H!G38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H40" s="478"/>
+      <c r="H40" s="477"/>
       <c r="I40" s="455"/>
-      <c r="J40" s="466" t="e">
+      <c r="J40" s="465" t="e">
         <f>EUR6_H!J38</f>
         <v>#DIV/0!</v>
       </c>
@@ -20579,9 +20657,9 @@
         <f>EUR6_H!G39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H41" s="478"/>
+      <c r="H41" s="477"/>
       <c r="I41" s="455"/>
-      <c r="J41" s="480" t="e">
+      <c r="J41" s="479" t="e">
         <f>EUR6_H!J39</f>
         <v>#DIV/0!</v>
       </c>
@@ -20597,287 +20675,287 @@
     </row>
     <row r="45" spans="1:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:10" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H46" s="481"/>
-      <c r="I46" s="520" t="s">
+      <c r="H46" s="480"/>
+      <c r="I46" s="528" t="s">
         <v>98</v>
       </c>
-      <c r="J46" s="521" t="str">
+      <c r="J46" s="529" t="str">
         <f>J11</f>
         <v>Part du TJM</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H47" s="482"/>
-      <c r="I47" s="520"/>
-      <c r="J47" s="521"/>
+      <c r="H47" s="481"/>
+      <c r="I47" s="528"/>
+      <c r="J47" s="529"/>
     </row>
     <row r="48" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H48" s="482"/>
-      <c r="I48" s="462" t="s">
+      <c r="H48" s="481"/>
+      <c r="I48" s="461" t="s">
         <v>26</v>
       </c>
-      <c r="J48" s="463" t="e">
+      <c r="J48" s="462" t="e">
         <f>EUR6_H!J45</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="49" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H49" s="482"/>
-      <c r="I49" s="464" t="s">
+      <c r="H49" s="481"/>
+      <c r="I49" s="463" t="s">
         <v>27</v>
       </c>
-      <c r="J49" s="465" t="e">
+      <c r="J49" s="464" t="e">
         <f>EUR6_H!J46</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="50" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H50" s="482"/>
-      <c r="I50" s="464" t="s">
+      <c r="H50" s="481"/>
+      <c r="I50" s="463" t="s">
         <v>28</v>
       </c>
-      <c r="J50" s="465" t="e">
+      <c r="J50" s="464" t="e">
         <f>EUR6_H!J47</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="51" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H51" s="482"/>
-      <c r="I51" s="464" t="s">
+      <c r="H51" s="481"/>
+      <c r="I51" s="463" t="s">
         <v>29</v>
       </c>
-      <c r="J51" s="465" t="e">
+      <c r="J51" s="464" t="e">
         <f>EUR6_H!J48</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="52" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H52" s="482"/>
-      <c r="I52" s="464" t="s">
+      <c r="H52" s="481"/>
+      <c r="I52" s="463" t="s">
         <v>30</v>
       </c>
-      <c r="J52" s="465" t="e">
+      <c r="J52" s="464" t="e">
         <f>EUR6_H!J49</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="53" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H53" s="482"/>
-      <c r="I53" s="464" t="s">
+      <c r="H53" s="481"/>
+      <c r="I53" s="463" t="s">
         <v>31</v>
       </c>
-      <c r="J53" s="465" t="e">
+      <c r="J53" s="464" t="e">
         <f>EUR6_H!J50</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="54" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H54" s="482"/>
-      <c r="I54" s="464" t="s">
+      <c r="H54" s="481"/>
+      <c r="I54" s="463" t="s">
         <v>32</v>
       </c>
-      <c r="J54" s="465" t="e">
+      <c r="J54" s="464" t="e">
         <f>EUR6_H!J51</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="55" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H55" s="482"/>
+      <c r="H55" s="481"/>
       <c r="I55" s="435" t="s">
         <v>33</v>
       </c>
-      <c r="J55" s="466" t="e">
+      <c r="J55" s="465" t="e">
         <f>EUR6_H!J52</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="56" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H56" s="482"/>
-      <c r="I56" s="464" t="s">
+      <c r="H56" s="481"/>
+      <c r="I56" s="463" t="s">
         <v>34</v>
       </c>
-      <c r="J56" s="465" t="e">
+      <c r="J56" s="464" t="e">
         <f>EUR6_H!J53</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="57" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H57" s="482"/>
-      <c r="I57" s="464" t="s">
+      <c r="H57" s="481"/>
+      <c r="I57" s="463" t="s">
         <v>35</v>
       </c>
-      <c r="J57" s="465" t="e">
+      <c r="J57" s="464" t="e">
         <f>EUR6_H!J54</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="58" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H58" s="482"/>
-      <c r="I58" s="464" t="s">
+      <c r="H58" s="481"/>
+      <c r="I58" s="463" t="s">
         <v>36</v>
       </c>
-      <c r="J58" s="465" t="e">
+      <c r="J58" s="464" t="e">
         <f>EUR6_H!J55</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="59" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H59" s="482"/>
-      <c r="I59" s="464" t="s">
+      <c r="H59" s="481"/>
+      <c r="I59" s="463" t="s">
         <v>37</v>
       </c>
-      <c r="J59" s="465" t="e">
+      <c r="J59" s="464" t="e">
         <f>EUR6_H!J56</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="60" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H60" s="482"/>
-      <c r="I60" s="467" t="s">
+      <c r="H60" s="481"/>
+      <c r="I60" s="466" t="s">
         <v>38</v>
       </c>
-      <c r="J60" s="465" t="e">
+      <c r="J60" s="464" t="e">
         <f>EUR6_H!J57</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="61" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H61" s="482"/>
-      <c r="I61" s="464" t="s">
+      <c r="H61" s="481"/>
+      <c r="I61" s="463" t="s">
         <v>39</v>
       </c>
-      <c r="J61" s="465" t="e">
+      <c r="J61" s="464" t="e">
         <f>EUR6_H!J58</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="62" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H62" s="482"/>
-      <c r="I62" s="464" t="s">
+      <c r="H62" s="481"/>
+      <c r="I62" s="463" t="s">
         <v>40</v>
       </c>
-      <c r="J62" s="465" t="e">
+      <c r="J62" s="464" t="e">
         <f>EUR6_H!J59</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="63" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H63" s="482"/>
-      <c r="I63" s="464" t="s">
+      <c r="H63" s="481"/>
+      <c r="I63" s="463" t="s">
         <v>41</v>
       </c>
-      <c r="J63" s="465" t="e">
+      <c r="J63" s="464" t="e">
         <f>EUR6_H!J60</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="64" spans="8:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H64" s="482"/>
-      <c r="I64" s="464" t="s">
+      <c r="H64" s="481"/>
+      <c r="I64" s="463" t="s">
         <v>42</v>
       </c>
-      <c r="J64" s="465" t="e">
+      <c r="J64" s="464" t="e">
         <f>EUR6_H!J61</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H65" s="482"/>
+      <c r="H65" s="481"/>
       <c r="I65" s="435" t="s">
         <v>43</v>
       </c>
-      <c r="J65" s="466" t="e">
+      <c r="J65" s="465" t="e">
         <f>EUR6_H!J62</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H66" s="482"/>
-      <c r="I66" s="464" t="s">
+      <c r="H66" s="481"/>
+      <c r="I66" s="463" t="s">
         <v>44</v>
       </c>
-      <c r="J66" s="465" t="e">
+      <c r="J66" s="464" t="e">
         <f>EUR6_H!J63</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H67" s="482"/>
-      <c r="I67" s="464" t="s">
+      <c r="H67" s="481"/>
+      <c r="I67" s="463" t="s">
         <v>45</v>
       </c>
-      <c r="J67" s="465" t="e">
+      <c r="J67" s="464" t="e">
         <f>EUR6_H!J64</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H68" s="482"/>
-      <c r="I68" s="464" t="s">
+      <c r="H68" s="481"/>
+      <c r="I68" s="463" t="s">
         <v>46</v>
       </c>
-      <c r="J68" s="465" t="e">
+      <c r="J68" s="464" t="e">
         <f>EUR6_H!J65</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H69" s="482"/>
-      <c r="I69" s="464" t="s">
+      <c r="H69" s="481"/>
+      <c r="I69" s="463" t="s">
         <v>47</v>
       </c>
-      <c r="J69" s="465" t="e">
+      <c r="J69" s="464" t="e">
         <f>EUR6_H!J66</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H70" s="482"/>
-      <c r="I70" s="464" t="s">
+      <c r="H70" s="481"/>
+      <c r="I70" s="463" t="s">
         <v>48</v>
       </c>
-      <c r="J70" s="465" t="e">
+      <c r="J70" s="464" t="e">
         <f>EUR6_H!J67</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H71" s="483"/>
+      <c r="H71" s="482"/>
       <c r="I71" s="418" t="s">
         <v>49</v>
       </c>
-      <c r="J71" s="469" t="e">
+      <c r="J71" s="468" t="e">
         <f>EUR6_H!J68</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H72" s="409"/>
-      <c r="I72" s="470"/>
-      <c r="J72" s="471"/>
+      <c r="I72" s="469"/>
+      <c r="J72" s="470"/>
     </row>
     <row r="73" spans="1:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="472" t="str">
+      <c r="B73" s="471" t="str">
         <f t="shared" ref="B73:G73" si="0">B38</f>
         <v>CAR (1)</v>
       </c>
-      <c r="C73" s="473" t="str">
+      <c r="C73" s="472" t="str">
         <f t="shared" si="0"/>
         <v>MR (2)</v>
       </c>
-      <c r="D73" s="474" t="str">
+      <c r="D73" s="473" t="str">
         <f t="shared" si="0"/>
         <v>PW (11)</v>
       </c>
-      <c r="E73" s="475" t="str">
+      <c r="E73" s="474" t="str">
         <f t="shared" si="0"/>
         <v>LIE (12)</v>
       </c>
-      <c r="F73" s="476" t="str">
+      <c r="F73" s="475" t="str">
         <f t="shared" si="0"/>
         <v>LW (8)</v>
       </c>
-      <c r="G73" s="477" t="str">
+      <c r="G73" s="476" t="str">
         <f t="shared" si="0"/>
         <v>LZ (9)</v>
       </c>
@@ -20910,9 +20988,9 @@
         <f>EUR6_H!G69</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H74" s="478"/>
+      <c r="H74" s="477"/>
       <c r="I74" s="455"/>
-      <c r="J74" s="479" t="e">
+      <c r="J74" s="478" t="e">
         <f>EUR6_H!J69</f>
         <v>#DIV/0!</v>
       </c>
@@ -20945,9 +21023,9 @@
         <f>EUR6_H!G70</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H75" s="478"/>
+      <c r="H75" s="477"/>
       <c r="I75" s="455"/>
-      <c r="J75" s="466" t="e">
+      <c r="J75" s="465" t="e">
         <f>EUR6_H!J70</f>
         <v>#DIV/0!</v>
       </c>
@@ -20980,9 +21058,9 @@
         <f>EUR6_H!G71</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H76" s="478"/>
+      <c r="H76" s="477"/>
       <c r="I76" s="455"/>
-      <c r="J76" s="480" t="e">
+      <c r="J76" s="479" t="e">
         <f>EUR6_H!J71</f>
         <v>#DIV/0!</v>
       </c>
@@ -21143,38 +21221,38 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="522"/>
-      <c r="B11" s="522"/>
-      <c r="C11" s="522"/>
-      <c r="D11" s="522"/>
-      <c r="E11" s="522"/>
-      <c r="F11" s="522"/>
-      <c r="G11" s="522"/>
-      <c r="H11" s="522"/>
-      <c r="I11" s="522"/>
-      <c r="J11" s="522"/>
-      <c r="K11" s="522"/>
-      <c r="L11" s="522"/>
-      <c r="M11" s="522"/>
-      <c r="N11" s="522"/>
-      <c r="O11" s="522"/>
+      <c r="A11" s="530"/>
+      <c r="B11" s="530"/>
+      <c r="C11" s="530"/>
+      <c r="D11" s="530"/>
+      <c r="E11" s="530"/>
+      <c r="F11" s="530"/>
+      <c r="G11" s="530"/>
+      <c r="H11" s="530"/>
+      <c r="I11" s="530"/>
+      <c r="J11" s="530"/>
+      <c r="K11" s="530"/>
+      <c r="L11" s="530"/>
+      <c r="M11" s="530"/>
+      <c r="N11" s="530"/>
+      <c r="O11" s="530"/>
     </row>
     <row r="12" spans="1:15" s="5" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="486" t="str">
+      <c r="B12" s="494" t="str">
         <f>"Distribution de la Vitesse par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)"</f>
         <v>Distribution de la Vitesse par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)</v>
       </c>
-      <c r="C12" s="486"/>
-      <c r="D12" s="486"/>
-      <c r="E12" s="486"/>
-      <c r="F12" s="486"/>
-      <c r="G12" s="486"/>
-      <c r="H12" s="486"/>
-      <c r="I12" s="486"/>
-      <c r="J12" s="486"/>
-      <c r="K12" s="486"/>
-      <c r="L12" s="486"/>
-      <c r="M12" s="486"/>
+      <c r="C12" s="494"/>
+      <c r="D12" s="494"/>
+      <c r="E12" s="494"/>
+      <c r="F12" s="494"/>
+      <c r="G12" s="494"/>
+      <c r="H12" s="494"/>
+      <c r="I12" s="494"/>
+      <c r="J12" s="494"/>
+      <c r="K12" s="494"/>
+      <c r="L12" s="494"/>
+      <c r="M12" s="494"/>
       <c r="N12" s="233"/>
       <c r="O12" s="234" t="s">
         <v>108</v>
@@ -22789,39 +22867,39 @@
       </c>
     </row>
     <row r="46" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="522"/>
-      <c r="B46" s="522"/>
-      <c r="C46" s="522"/>
-      <c r="D46" s="522"/>
-      <c r="E46" s="522"/>
-      <c r="F46" s="522"/>
-      <c r="G46" s="522"/>
-      <c r="H46" s="522"/>
-      <c r="I46" s="522"/>
-      <c r="J46" s="522"/>
-      <c r="K46" s="522"/>
-      <c r="L46" s="522"/>
-      <c r="M46" s="522"/>
-      <c r="N46" s="522"/>
-      <c r="O46" s="522"/>
+      <c r="A46" s="530"/>
+      <c r="B46" s="530"/>
+      <c r="C46" s="530"/>
+      <c r="D46" s="530"/>
+      <c r="E46" s="530"/>
+      <c r="F46" s="530"/>
+      <c r="G46" s="530"/>
+      <c r="H46" s="530"/>
+      <c r="I46" s="530"/>
+      <c r="J46" s="530"/>
+      <c r="K46" s="530"/>
+      <c r="L46" s="530"/>
+      <c r="M46" s="530"/>
+      <c r="N46" s="530"/>
+      <c r="O46" s="530"/>
     </row>
     <row r="47" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
-      <c r="B47" s="486" t="str">
+      <c r="B47" s="494" t="str">
         <f>B12</f>
         <v>Distribution de la Vitesse par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)</v>
       </c>
-      <c r="C47" s="486"/>
-      <c r="D47" s="486"/>
-      <c r="E47" s="486"/>
-      <c r="F47" s="486"/>
-      <c r="G47" s="486"/>
-      <c r="H47" s="486"/>
-      <c r="I47" s="486"/>
-      <c r="J47" s="486"/>
-      <c r="K47" s="486"/>
-      <c r="L47" s="486"/>
-      <c r="M47" s="486"/>
+      <c r="C47" s="494"/>
+      <c r="D47" s="494"/>
+      <c r="E47" s="494"/>
+      <c r="F47" s="494"/>
+      <c r="G47" s="494"/>
+      <c r="H47" s="494"/>
+      <c r="I47" s="494"/>
+      <c r="J47" s="494"/>
+      <c r="K47" s="494"/>
+      <c r="L47" s="494"/>
+      <c r="M47" s="494"/>
       <c r="N47" s="233"/>
       <c r="O47" s="234" t="str">
         <f>O12</f>
@@ -24585,59 +24663,59 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="522" t="str">
+      <c r="A11" s="530" t="str">
         <f>"Vitesse moyenne = "&amp;INT(U39)&amp;" km/h"</f>
         <v>Vitesse moyenne = 0 km/h</v>
       </c>
-      <c r="B11" s="522"/>
-      <c r="C11" s="522"/>
-      <c r="D11" s="522"/>
-      <c r="E11" s="522"/>
-      <c r="F11" s="522"/>
-      <c r="G11" s="522"/>
-      <c r="H11" s="522"/>
-      <c r="I11" s="522"/>
-      <c r="J11" s="522"/>
-      <c r="K11" s="522"/>
-      <c r="L11" s="522"/>
-      <c r="M11" s="522"/>
-      <c r="N11" s="522"/>
-      <c r="O11" s="522"/>
-      <c r="P11" s="522"/>
-      <c r="Q11" s="522"/>
-      <c r="R11" s="522"/>
-      <c r="S11" s="522"/>
-      <c r="T11" s="522"/>
-      <c r="U11" s="522"/>
+      <c r="B11" s="530"/>
+      <c r="C11" s="530"/>
+      <c r="D11" s="530"/>
+      <c r="E11" s="530"/>
+      <c r="F11" s="530"/>
+      <c r="G11" s="530"/>
+      <c r="H11" s="530"/>
+      <c r="I11" s="530"/>
+      <c r="J11" s="530"/>
+      <c r="K11" s="530"/>
+      <c r="L11" s="530"/>
+      <c r="M11" s="530"/>
+      <c r="N11" s="530"/>
+      <c r="O11" s="530"/>
+      <c r="P11" s="530"/>
+      <c r="Q11" s="530"/>
+      <c r="R11" s="530"/>
+      <c r="S11" s="530"/>
+      <c r="T11" s="530"/>
+      <c r="U11" s="530"/>
     </row>
     <row r="12" spans="1:21" s="5" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="486" t="str">
+      <c r="B12" s="494" t="str">
         <f>"Distribution de la Vitesse par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)"</f>
         <v>Distribution de la Vitesse par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)</v>
       </c>
-      <c r="C12" s="486"/>
-      <c r="D12" s="486"/>
-      <c r="E12" s="486"/>
-      <c r="F12" s="486"/>
-      <c r="G12" s="486"/>
-      <c r="H12" s="486"/>
-      <c r="I12" s="486"/>
-      <c r="J12" s="486"/>
-      <c r="K12" s="486"/>
-      <c r="L12" s="486"/>
-      <c r="M12" s="486"/>
-      <c r="N12" s="486"/>
+      <c r="C12" s="494"/>
+      <c r="D12" s="494"/>
+      <c r="E12" s="494"/>
+      <c r="F12" s="494"/>
+      <c r="G12" s="494"/>
+      <c r="H12" s="494"/>
+      <c r="I12" s="494"/>
+      <c r="J12" s="494"/>
+      <c r="K12" s="494"/>
+      <c r="L12" s="494"/>
+      <c r="M12" s="494"/>
+      <c r="N12" s="494"/>
       <c r="O12" s="233"/>
       <c r="P12" s="234" t="s">
         <v>108</v>
       </c>
       <c r="Q12" s="305"/>
-      <c r="R12" s="486" t="s">
+      <c r="R12" s="494" t="s">
         <v>155</v>
       </c>
-      <c r="S12" s="486"/>
-      <c r="T12" s="486"/>
-      <c r="U12" s="486"/>
+      <c r="S12" s="494"/>
+      <c r="T12" s="494"/>
+      <c r="U12" s="494"/>
     </row>
     <row r="13" spans="1:21" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="123" t="s">
@@ -26844,62 +26922,62 @@
       <c r="U45" s="6"/>
     </row>
     <row r="46" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="522" t="str">
+      <c r="A46" s="530" t="str">
         <f>"Vitesse moyenne = "&amp;INT(U74)&amp;" km/h"</f>
         <v>Vitesse moyenne = 0 km/h</v>
       </c>
-      <c r="B46" s="522"/>
-      <c r="C46" s="522"/>
-      <c r="D46" s="522"/>
-      <c r="E46" s="522"/>
-      <c r="F46" s="522"/>
-      <c r="G46" s="522"/>
-      <c r="H46" s="522"/>
-      <c r="I46" s="522"/>
-      <c r="J46" s="522"/>
-      <c r="K46" s="522"/>
-      <c r="L46" s="522"/>
-      <c r="M46" s="522"/>
-      <c r="N46" s="522"/>
-      <c r="O46" s="522"/>
-      <c r="P46" s="522"/>
-      <c r="Q46" s="522"/>
-      <c r="R46" s="522"/>
-      <c r="S46" s="522"/>
-      <c r="T46" s="522"/>
-      <c r="U46" s="522"/>
+      <c r="B46" s="530"/>
+      <c r="C46" s="530"/>
+      <c r="D46" s="530"/>
+      <c r="E46" s="530"/>
+      <c r="F46" s="530"/>
+      <c r="G46" s="530"/>
+      <c r="H46" s="530"/>
+      <c r="I46" s="530"/>
+      <c r="J46" s="530"/>
+      <c r="K46" s="530"/>
+      <c r="L46" s="530"/>
+      <c r="M46" s="530"/>
+      <c r="N46" s="530"/>
+      <c r="O46" s="530"/>
+      <c r="P46" s="530"/>
+      <c r="Q46" s="530"/>
+      <c r="R46" s="530"/>
+      <c r="S46" s="530"/>
+      <c r="T46" s="530"/>
+      <c r="U46" s="530"/>
     </row>
     <row r="47" spans="1:21" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
-      <c r="B47" s="486" t="str">
+      <c r="B47" s="494" t="str">
         <f>B12</f>
         <v>Distribution de la Vitesse par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)</v>
       </c>
-      <c r="C47" s="486"/>
-      <c r="D47" s="486"/>
-      <c r="E47" s="486"/>
-      <c r="F47" s="486"/>
-      <c r="G47" s="486"/>
-      <c r="H47" s="486"/>
-      <c r="I47" s="486"/>
-      <c r="J47" s="486"/>
-      <c r="K47" s="486"/>
-      <c r="L47" s="486"/>
-      <c r="M47" s="486"/>
-      <c r="N47" s="486"/>
+      <c r="C47" s="494"/>
+      <c r="D47" s="494"/>
+      <c r="E47" s="494"/>
+      <c r="F47" s="494"/>
+      <c r="G47" s="494"/>
+      <c r="H47" s="494"/>
+      <c r="I47" s="494"/>
+      <c r="J47" s="494"/>
+      <c r="K47" s="494"/>
+      <c r="L47" s="494"/>
+      <c r="M47" s="494"/>
+      <c r="N47" s="494"/>
       <c r="O47" s="233"/>
       <c r="P47" s="234" t="str">
         <f>P12</f>
         <v>THM</v>
       </c>
       <c r="Q47" s="305"/>
-      <c r="R47" s="486" t="str">
+      <c r="R47" s="494" t="str">
         <f>R12</f>
         <v>Vitesses caractéristiques</v>
       </c>
-      <c r="S47" s="486"/>
-      <c r="T47" s="486"/>
-      <c r="U47" s="486"/>
+      <c r="S47" s="494"/>
+      <c r="T47" s="494"/>
+      <c r="U47" s="494"/>
     </row>
     <row r="48" spans="1:21" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="123" t="s">
@@ -29183,12 +29261,12 @@
       <c r="H2" s="4">
         <v>0</v>
       </c>
-      <c r="M2" s="485" t="s">
-        <v>199</v>
-      </c>
-      <c r="N2" s="485"/>
-      <c r="O2" s="485"/>
-      <c r="P2" s="485"/>
+      <c r="M2" s="493" t="s">
+        <v>198</v>
+      </c>
+      <c r="N2" s="493"/>
+      <c r="O2" s="493"/>
+      <c r="P2" s="493"/>
     </row>
     <row r="3" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -29230,11 +29308,11 @@
         <v>16</v>
       </c>
       <c r="M3" s="394"/>
-      <c r="N3" s="485" t="s">
-        <v>195</v>
-      </c>
-      <c r="O3" s="485"/>
-      <c r="P3" s="485"/>
+      <c r="N3" s="493" t="s">
+        <v>194</v>
+      </c>
+      <c r="O3" s="493"/>
+      <c r="P3" s="493"/>
     </row>
     <row r="4" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="379" t="s">
@@ -29269,13 +29347,13 @@
       </c>
       <c r="M4" s="394"/>
       <c r="N4" s="394" t="s">
+        <v>199</v>
+      </c>
+      <c r="O4" s="394" t="s">
         <v>200</v>
       </c>
-      <c r="O4" s="394" t="s">
+      <c r="P4" s="394" t="s">
         <v>201</v>
-      </c>
-      <c r="P4" s="394" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
@@ -29369,7 +29447,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M6" s="394" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N6" s="394"/>
       <c r="O6" s="394">
@@ -29419,7 +29497,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M7" s="394" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N7" s="394"/>
       <c r="O7" s="394" t="e">
@@ -29511,7 +29589,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M9" s="394" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N9" s="394">
         <f>I60</f>
@@ -29564,7 +29642,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M10" s="394" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N10" s="394"/>
       <c r="O10" s="394">
@@ -29614,7 +29692,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M11" s="394" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N11" s="394"/>
       <c r="O11" s="394" t="e">
@@ -29753,7 +29831,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M14" s="394" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N14" s="394"/>
       <c r="O14" s="394"/>
@@ -29797,7 +29875,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M15" s="394" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N15" s="394"/>
       <c r="O15" s="394"/>
@@ -29878,8 +29956,8 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M17" s="484" t="s">
-        <v>204</v>
+      <c r="M17" s="483" t="s">
+        <v>203</v>
       </c>
       <c r="N17" s="394">
         <f>N13/7</f>
@@ -30427,7 +30505,7 @@
     </row>
     <row r="32" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B32" s="10" t="e">
         <f>B31/B29</f>
@@ -31585,7 +31663,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B63" s="10" t="e">
         <f>B62/B60</f>
@@ -32978,7 +33056,7 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B94" s="10" t="e">
         <f>B93/B91</f>
@@ -40604,7 +40682,7 @@
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A62" s="389" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B62" s="390"/>
       <c r="C62" s="391"/>
@@ -40628,7 +40706,7 @@
     <row r="63" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A63" s="390"/>
       <c r="B63" s="390" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C63" s="390" t="s">
         <v>112</v>
@@ -40672,7 +40750,7 @@
     <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64" s="390"/>
       <c r="B64" s="390" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C64" s="390">
         <v>1</v>
@@ -40704,7 +40782,7 @@
       <c r="L64" s="390">
         <v>10</v>
       </c>
-      <c r="M64" s="392"/>
+      <c r="M64" s="492"/>
       <c r="T64"/>
       <c r="U64"/>
       <c r="V64"/>
@@ -40746,7 +40824,7 @@
       <c r="L65" s="390">
         <v>1</v>
       </c>
-      <c r="M65" s="392"/>
+      <c r="M65" s="492"/>
       <c r="S65"/>
       <c r="T65"/>
       <c r="U65"/>
@@ -40757,7 +40835,7 @@
     <row r="66" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A66" s="390"/>
       <c r="B66" s="390" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C66" s="390">
         <f>C$65*SUM(C$39:C$54,C$11:C$26)</f>
@@ -40799,7 +40877,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="M66" s="392">
+      <c r="M66" s="492">
         <f>SUM(C66:L66)</f>
         <v>0</v>
       </c>
@@ -40813,7 +40891,7 @@
     <row r="67" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A67" s="390"/>
       <c r="B67" s="390" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C67" s="390">
         <f>C$65*SUM(C$33:C$38,C$55:C$56,C$5:C$10,C$27:C$28)</f>
@@ -40855,7 +40933,7 @@
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="M67" s="392">
+      <c r="M67" s="492">
         <f t="shared" ref="M67:M70" si="28">SUM(C67:L67)</f>
         <v>0</v>
       </c>
@@ -40899,7 +40977,7 @@
       <c r="L68" s="390">
         <v>0</v>
       </c>
-      <c r="M68" s="392"/>
+      <c r="M68" s="492"/>
       <c r="U68"/>
       <c r="V68"/>
       <c r="W68"/>
@@ -40908,7 +40986,7 @@
     <row r="69" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A69" s="390"/>
       <c r="B69" s="390" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C69" s="390">
         <f>C$68*SUM(C$39:C$54,C$11:C$26)</f>
@@ -40950,7 +41028,7 @@
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="M69" s="392">
+      <c r="M69" s="492">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
@@ -40962,7 +41040,7 @@
     <row r="70" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A70" s="390"/>
       <c r="B70" s="390" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C70" s="390">
         <f>C$68*SUM(C$33:C$38,C$55:C$56,C$5:C$10,C$27:C$28)</f>
@@ -41004,7 +41082,7 @@
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="M70" s="392">
+      <c r="M70" s="492">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
@@ -41026,7 +41104,7 @@
       <c r="J71" s="390"/>
       <c r="K71" s="390"/>
       <c r="L71" s="390"/>
-      <c r="M71" s="392"/>
+      <c r="M71" s="492"/>
       <c r="U71"/>
       <c r="V71"/>
       <c r="W71"/>
@@ -41035,7 +41113,7 @@
     <row r="72" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A72" s="390"/>
       <c r="B72" s="390" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C72" s="390" t="s">
         <v>112</v>
@@ -41061,7 +41139,7 @@
       <c r="J72" s="390"/>
       <c r="K72" s="390"/>
       <c r="L72" s="390"/>
-      <c r="M72" s="392"/>
+      <c r="M72" s="492"/>
       <c r="U72"/>
       <c r="V72"/>
       <c r="W72"/>
@@ -41070,7 +41148,7 @@
     <row r="73" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A73" s="390"/>
       <c r="B73" s="390" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C73" s="390">
         <v>1</v>
@@ -41096,7 +41174,7 @@
       <c r="J73" s="390"/>
       <c r="K73" s="390"/>
       <c r="L73" s="390"/>
-      <c r="M73" s="392"/>
+      <c r="M73" s="492"/>
       <c r="U73"/>
       <c r="V73"/>
       <c r="W73"/>
@@ -41131,7 +41209,7 @@
       <c r="J74" s="390"/>
       <c r="K74" s="390"/>
       <c r="L74" s="390"/>
-      <c r="M74" s="392"/>
+      <c r="M74" s="492"/>
       <c r="U74"/>
       <c r="V74"/>
       <c r="W74"/>
@@ -41140,7 +41218,7 @@
     <row r="75" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A75" s="390"/>
       <c r="B75" s="390" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C75" s="390">
         <f>C$74*SUM(C$39:C$54,C$11:C$26)</f>
@@ -41173,7 +41251,7 @@
       <c r="J75" s="390"/>
       <c r="K75" s="390"/>
       <c r="L75" s="390"/>
-      <c r="M75" s="392">
+      <c r="M75" s="492">
         <f>SUM(C75:I75)</f>
         <v>0</v>
       </c>
@@ -41185,7 +41263,7 @@
     <row r="76" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A76" s="390"/>
       <c r="B76" s="390" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C76" s="390">
         <f>C$74*SUM(C$33:C$38,C$55:C$56,C$5:C$10,C$27:C$28)</f>
@@ -41218,8 +41296,8 @@
       <c r="J76" s="390"/>
       <c r="K76" s="390"/>
       <c r="L76" s="390"/>
-      <c r="M76" s="392">
-        <f t="shared" ref="M76:M106" si="33">SUM(C76:I76)</f>
+      <c r="M76" s="492">
+        <f t="shared" ref="M76:M88" si="33">SUM(C76:I76)</f>
         <v>0</v>
       </c>
       <c r="U76"/>
@@ -41256,7 +41334,7 @@
       <c r="J77" s="390"/>
       <c r="K77" s="390"/>
       <c r="L77" s="390"/>
-      <c r="M77" s="392"/>
+      <c r="M77" s="492"/>
       <c r="U77"/>
       <c r="V77"/>
       <c r="W77"/>
@@ -41265,7 +41343,7 @@
     <row r="78" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A78" s="390"/>
       <c r="B78" s="390" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C78" s="390">
         <f>C$77*SUM(C$39:C$54,C$11:C$26)</f>
@@ -41298,7 +41376,7 @@
       <c r="J78" s="390"/>
       <c r="K78" s="390"/>
       <c r="L78" s="390"/>
-      <c r="M78" s="392">
+      <c r="M78" s="492">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
@@ -41310,7 +41388,7 @@
     <row r="79" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A79" s="390"/>
       <c r="B79" s="390" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C79" s="390">
         <f>C$77*SUM(C$33:C$38,C$55:C$56,C$5:C$10,C$27:C$28)</f>
@@ -41343,7 +41421,7 @@
       <c r="J79" s="390"/>
       <c r="K79" s="390"/>
       <c r="L79" s="390"/>
-      <c r="M79" s="392">
+      <c r="M79" s="492">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
@@ -41365,7 +41443,7 @@
       <c r="J80" s="390"/>
       <c r="K80" s="390"/>
       <c r="L80" s="390"/>
-      <c r="M80" s="392"/>
+      <c r="M80" s="492"/>
       <c r="U80"/>
       <c r="V80"/>
       <c r="W80"/>
@@ -41374,7 +41452,7 @@
     <row r="81" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A81" s="390"/>
       <c r="B81" s="390" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C81" s="390" t="s">
         <v>112</v>
@@ -41400,7 +41478,7 @@
       <c r="J81" s="390"/>
       <c r="K81" s="390"/>
       <c r="L81" s="390"/>
-      <c r="M81" s="392"/>
+      <c r="M81" s="492"/>
       <c r="U81"/>
       <c r="V81"/>
       <c r="W81"/>
@@ -41409,7 +41487,7 @@
     <row r="82" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A82" s="390"/>
       <c r="B82" s="390" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C82" s="390">
         <v>1</v>
@@ -41435,7 +41513,7 @@
       <c r="J82" s="390"/>
       <c r="K82" s="390"/>
       <c r="L82" s="390"/>
-      <c r="M82" s="392"/>
+      <c r="M82" s="492"/>
       <c r="U82"/>
       <c r="V82"/>
       <c r="W82"/>
@@ -41470,7 +41548,7 @@
       <c r="J83" s="390"/>
       <c r="K83" s="390"/>
       <c r="L83" s="390"/>
-      <c r="M83" s="392"/>
+      <c r="M83" s="492"/>
       <c r="U83"/>
       <c r="V83"/>
       <c r="W83"/>
@@ -41479,7 +41557,7 @@
     <row r="84" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A84" s="390"/>
       <c r="B84" s="390" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C84" s="390">
         <f>C$83*SUM(C$39:C$54,C$11:C$26)</f>
@@ -41512,7 +41590,7 @@
       <c r="J84" s="390"/>
       <c r="K84" s="390"/>
       <c r="L84" s="390"/>
-      <c r="M84" s="392">
+      <c r="M84" s="492">
         <f>SUM(C84:I84)</f>
         <v>0</v>
       </c>
@@ -41524,7 +41602,7 @@
     <row r="85" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A85" s="390"/>
       <c r="B85" s="390" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C85" s="390">
         <f>C$83*SUM(C$33:C$38,C$55:C$56,C$5:C$10,C$27:C$28)</f>
@@ -41557,7 +41635,7 @@
       <c r="J85" s="390"/>
       <c r="K85" s="390"/>
       <c r="L85" s="390"/>
-      <c r="M85" s="392">
+      <c r="M85" s="492">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
@@ -41595,7 +41673,7 @@
       <c r="J86" s="390"/>
       <c r="K86" s="390"/>
       <c r="L86" s="390"/>
-      <c r="M86" s="392"/>
+      <c r="M86" s="492"/>
       <c r="U86"/>
       <c r="V86"/>
       <c r="W86"/>
@@ -41604,7 +41682,7 @@
     <row r="87" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A87" s="390"/>
       <c r="B87" s="390" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C87" s="390">
         <f>C$86*SUM(C$39:C$54,C$11:C$26)</f>
@@ -41637,7 +41715,7 @@
       <c r="J87" s="390"/>
       <c r="K87" s="390"/>
       <c r="L87" s="390"/>
-      <c r="M87" s="392">
+      <c r="M87" s="492">
         <f>SUM(C87:I87)</f>
         <v>0</v>
       </c>
@@ -41649,7 +41727,7 @@
     <row r="88" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A88" s="390"/>
       <c r="B88" s="390" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C88" s="390">
         <f>C$86*SUM(C$33:C$38,C$55:C$56,C$5:C$10,C$27:C$28)</f>
@@ -41682,7 +41760,7 @@
       <c r="J88" s="390"/>
       <c r="K88" s="390"/>
       <c r="L88" s="390"/>
-      <c r="M88" s="392">
+      <c r="M88" s="492">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
@@ -41704,7 +41782,7 @@
       <c r="J89" s="390"/>
       <c r="K89" s="390"/>
       <c r="L89" s="390"/>
-      <c r="M89" s="392"/>
+      <c r="M89" s="492"/>
       <c r="U89"/>
       <c r="V89"/>
       <c r="W89"/>
@@ -41713,31 +41791,31 @@
     <row r="90" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A90" s="390"/>
       <c r="B90" s="390" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C90" s="390" t="s">
+        <v>112</v>
+      </c>
+      <c r="D90" s="390" t="s">
         <v>113</v>
       </c>
-      <c r="D90" s="390" t="s">
+      <c r="E90" s="390" t="s">
         <v>171</v>
       </c>
-      <c r="E90" s="390" t="s">
+      <c r="F90" s="390" t="s">
         <v>168</v>
       </c>
-      <c r="F90" s="390" t="s">
+      <c r="G90" s="390" t="s">
         <v>172</v>
       </c>
-      <c r="G90" s="390" t="s">
+      <c r="H90" s="390" t="s">
         <v>173</v>
-      </c>
-      <c r="H90" s="390" t="s">
-        <v>112</v>
       </c>
       <c r="I90" s="390"/>
       <c r="J90" s="390"/>
       <c r="K90" s="390"/>
       <c r="L90" s="390"/>
-      <c r="M90" s="392"/>
+      <c r="M90" s="492"/>
       <c r="U90"/>
       <c r="V90"/>
       <c r="W90"/>
@@ -41746,7 +41824,7 @@
     <row r="91" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A91" s="390"/>
       <c r="B91" s="390" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C91" s="390">
         <v>1</v>
@@ -41770,7 +41848,7 @@
       <c r="J91" s="390"/>
       <c r="K91" s="390"/>
       <c r="L91" s="390"/>
-      <c r="M91" s="392"/>
+      <c r="M91" s="492"/>
       <c r="U91"/>
       <c r="V91"/>
       <c r="W91"/>
@@ -41785,13 +41863,13 @@
         <v>1</v>
       </c>
       <c r="D92" s="390">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92" s="390">
         <v>0</v>
       </c>
       <c r="F92" s="390">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G92" s="390">
         <v>1</v>
@@ -41803,7 +41881,7 @@
       <c r="J92" s="390"/>
       <c r="K92" s="390"/>
       <c r="L92" s="390"/>
-      <c r="M92" s="392"/>
+      <c r="M92" s="492"/>
       <c r="U92"/>
       <c r="V92"/>
       <c r="W92"/>
@@ -41812,7 +41890,7 @@
     <row r="93" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A93" s="390"/>
       <c r="B93" s="390" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C93" s="390">
         <f>C$92*SUM(C$39:C$54,C$11:C$26)</f>
@@ -41842,7 +41920,7 @@
       <c r="J93" s="390"/>
       <c r="K93" s="390"/>
       <c r="L93" s="390"/>
-      <c r="M93" s="392">
+      <c r="M93" s="492">
         <f>SUM(C93:H93)</f>
         <v>0</v>
       </c>
@@ -41854,14 +41932,14 @@
     <row r="94" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A94" s="390"/>
       <c r="B94" s="390" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C94" s="390">
-        <f>C$92*SUM(C$33:C$38,C$55:C$56,C$5:C$10,C$27:C$28)</f>
+        <f t="shared" ref="C94:H94" si="41">C$92*SUM(C$33:C$38,C$55:C$56,C$5:C$10,C$27:C$28)</f>
         <v>0</v>
       </c>
       <c r="D94" s="390">
-        <f t="shared" ref="D94:H94" si="41">D$92*SUM(D$33:D$38,D$55:D$56,D$5:D$10,D$27:D$28)</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="E94" s="390">
@@ -41884,8 +41962,8 @@
       <c r="J94" s="390"/>
       <c r="K94" s="390"/>
       <c r="L94" s="390"/>
-      <c r="M94" s="392">
-        <f t="shared" ref="M94:M97" si="42">SUM(C94:H94)</f>
+      <c r="M94" s="492">
+        <f>SUM(C94:H94)</f>
         <v>0</v>
       </c>
       <c r="U94"/>
@@ -41902,13 +41980,13 @@
         <v>0</v>
       </c>
       <c r="D95" s="390">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E95" s="390">
         <v>1</v>
       </c>
       <c r="F95" s="390">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G95" s="390">
         <v>0</v>
@@ -41920,7 +41998,7 @@
       <c r="J95" s="390"/>
       <c r="K95" s="390"/>
       <c r="L95" s="390"/>
-      <c r="M95" s="392"/>
+      <c r="M95" s="492"/>
       <c r="U95"/>
       <c r="V95"/>
       <c r="W95"/>
@@ -41929,37 +42007,37 @@
     <row r="96" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A96" s="390"/>
       <c r="B96" s="390" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C96" s="390">
-        <f>C$95*SUM(C$39:C$54,C$11:C$26)</f>
+        <f t="shared" ref="C96:H96" si="42">C$95*SUM(C$39:C$54,C$11:C$26)</f>
         <v>0</v>
       </c>
       <c r="D96" s="390">
-        <f t="shared" ref="D96:H96" si="43">D$95*SUM(D$39:D$54,D$11:D$26)</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="E96" s="390">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="F96" s="390">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G96" s="390">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="H96" s="390">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="I96" s="390"/>
       <c r="J96" s="390"/>
       <c r="K96" s="390"/>
       <c r="L96" s="390"/>
-      <c r="M96" s="392">
+      <c r="M96" s="492">
         <f>SUM(C96:H96)</f>
         <v>0</v>
       </c>
@@ -41971,38 +42049,38 @@
     <row r="97" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A97" s="390"/>
       <c r="B97" s="390" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C97" s="390">
-        <f>C$95*SUM(C$33:C$38,C$55:C$56,C$5:C$10,C$27:C$28)</f>
+        <f t="shared" ref="C97:H97" si="43">C$95*SUM(C$33:C$38,C$55:C$56,C$5:C$10,C$27:C$28)</f>
         <v>0</v>
       </c>
       <c r="D97" s="390">
-        <f t="shared" ref="D97:H97" si="44">D$95*SUM(D$33:D$38,D$55:D$56,D$5:D$10,D$27:D$28)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="E97" s="390">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="F97" s="390">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="G97" s="390">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="H97" s="390">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="I97" s="390"/>
       <c r="J97" s="390"/>
       <c r="K97" s="390"/>
       <c r="L97" s="390"/>
-      <c r="M97" s="392">
-        <f t="shared" si="42"/>
+      <c r="M97" s="492">
+        <f>SUM(C97:H97)</f>
         <v>0</v>
       </c>
       <c r="U97"/>
@@ -42023,7 +42101,7 @@
       <c r="J98" s="390"/>
       <c r="K98" s="390"/>
       <c r="L98" s="390"/>
-      <c r="M98" s="392"/>
+      <c r="M98" s="492"/>
       <c r="U98"/>
       <c r="V98"/>
       <c r="W98"/>
@@ -42035,13 +42113,13 @@
         <v>165</v>
       </c>
       <c r="C99" s="390" t="s">
+        <v>112</v>
+      </c>
+      <c r="D99" s="390" t="s">
         <v>171</v>
       </c>
-      <c r="D99" s="390" t="s">
-        <v>174</v>
-      </c>
       <c r="E99" s="390" t="s">
-        <v>112</v>
+        <v>205</v>
       </c>
       <c r="F99" s="390" t="s">
         <v>116</v>
@@ -42058,7 +42136,7 @@
       <c r="J99" s="390"/>
       <c r="K99" s="390"/>
       <c r="L99" s="390"/>
-      <c r="M99" s="392"/>
+      <c r="M99" s="492"/>
       <c r="U99"/>
       <c r="V99"/>
       <c r="W99"/>
@@ -42093,7 +42171,7 @@
       <c r="J100" s="390"/>
       <c r="K100" s="390"/>
       <c r="L100" s="390"/>
-      <c r="M100" s="392"/>
+      <c r="M100" s="492"/>
       <c r="U100"/>
       <c r="V100"/>
       <c r="W100"/>
@@ -42105,13 +42183,13 @@
         <v>166</v>
       </c>
       <c r="C101" s="390">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D101" s="390">
         <v>0</v>
       </c>
       <c r="E101" s="390">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F101" s="390">
         <v>1</v>
@@ -42128,7 +42206,7 @@
       <c r="J101" s="390"/>
       <c r="K101" s="390"/>
       <c r="L101" s="390"/>
-      <c r="M101" s="392"/>
+      <c r="M101" s="492"/>
       <c r="U101"/>
       <c r="V101"/>
       <c r="W101"/>
@@ -42137,40 +42215,40 @@
     <row r="102" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A102" s="390"/>
       <c r="B102" s="390" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C102" s="390">
-        <f t="shared" ref="C102:I102" si="45">C$101*SUM(C$39:C$54,C$11:C$26)</f>
+        <f t="shared" ref="C102:I102" si="44">C$101*SUM(C$39:C$54,C$11:C$26)</f>
         <v>0</v>
       </c>
       <c r="D102" s="390">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="E102" s="390">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="F102" s="390">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="G102" s="390">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="H102" s="390">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="I102" s="390">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="J102" s="390"/>
       <c r="K102" s="390"/>
       <c r="L102" s="390"/>
-      <c r="M102" s="392">
+      <c r="M102" s="492">
         <f>SUM(C102:I102)</f>
         <v>0</v>
       </c>
@@ -42182,41 +42260,41 @@
     <row r="103" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A103" s="390"/>
       <c r="B103" s="390" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C103" s="390">
-        <f t="shared" ref="C103:I103" si="46">C$101*SUM(C$33:C$38,C$55:C$56,C$5:C$10,C$27:C$28)</f>
+        <f t="shared" ref="C103:I103" si="45">C$101*SUM(C$33:C$38,C$55:C$56,C$5:C$10,C$27:C$28)</f>
         <v>0</v>
       </c>
       <c r="D103" s="390">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="E103" s="390">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="F103" s="390">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="G103" s="390">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="H103" s="390">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="I103" s="390">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="J103" s="390"/>
       <c r="K103" s="390"/>
       <c r="L103" s="390"/>
-      <c r="M103" s="392">
-        <f t="shared" si="33"/>
+      <c r="M103" s="492">
+        <f>SUM(C103:I103)</f>
         <v>0</v>
       </c>
       <c r="U103"/>
@@ -42230,13 +42308,13 @@
         <v>167</v>
       </c>
       <c r="C104" s="390">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D104" s="390">
         <v>1</v>
       </c>
       <c r="E104" s="390">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F104" s="390">
         <v>0</v>
@@ -42253,7 +42331,7 @@
       <c r="J104" s="390"/>
       <c r="K104" s="390"/>
       <c r="L104" s="390"/>
-      <c r="M104" s="392"/>
+      <c r="M104" s="492"/>
       <c r="U104"/>
       <c r="V104"/>
       <c r="W104"/>
@@ -42262,40 +42340,40 @@
     <row r="105" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A105" s="390"/>
       <c r="B105" s="390" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C105" s="390">
-        <f t="shared" ref="C105:I105" si="47">C$104*SUM(C$39:C$54,C$11:C$26)</f>
+        <f t="shared" ref="C105:I105" si="46">C$104*SUM(C$39:C$54,C$11:C$26)</f>
         <v>0</v>
       </c>
       <c r="D105" s="390">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="E105" s="390">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="F105" s="390">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="G105" s="390">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="H105" s="390">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="I105" s="390">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="J105" s="390"/>
       <c r="K105" s="390"/>
       <c r="L105" s="390"/>
-      <c r="M105" s="392">
+      <c r="M105" s="492">
         <f>SUM(C105:I105)</f>
         <v>0</v>
       </c>
@@ -42307,41 +42385,41 @@
     <row r="106" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A106" s="390"/>
       <c r="B106" s="390" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C106" s="390">
-        <f t="shared" ref="C106:I106" si="48">C$104*SUM(C$33:C$38,C$55:C$56,C$5:C$10,C$27:C$28)</f>
+        <f t="shared" ref="C106:I106" si="47">C$104*SUM(C$33:C$38,C$55:C$56,C$5:C$10,C$27:C$28)</f>
         <v>0</v>
       </c>
       <c r="D106" s="390">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="E106" s="390">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="F106" s="390">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="G106" s="390">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="H106" s="390">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="I106" s="390">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="J106" s="390"/>
       <c r="K106" s="390"/>
       <c r="L106" s="390"/>
-      <c r="M106" s="392">
-        <f t="shared" si="33"/>
+      <c r="M106" s="492">
+        <f>SUM(C106:I106)</f>
         <v>0</v>
       </c>
       <c r="U106"/>
@@ -42451,36 +42529,36 @@
       <c r="C8" s="18"/>
     </row>
     <row r="9" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="486" t="s">
+      <c r="C9" s="494" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="486"/>
-      <c r="E9" s="486"/>
-      <c r="F9" s="486"/>
-      <c r="G9" s="486"/>
-      <c r="H9" s="486"/>
-      <c r="I9" s="486"/>
-      <c r="J9" s="486"/>
-      <c r="K9" s="486"/>
+      <c r="D9" s="494"/>
+      <c r="E9" s="494"/>
+      <c r="F9" s="494"/>
+      <c r="G9" s="494"/>
+      <c r="H9" s="494"/>
+      <c r="I9" s="494"/>
+      <c r="J9" s="494"/>
+      <c r="K9" s="494"/>
     </row>
     <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="487" t="s">
+      <c r="C10" s="495" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="487"/>
-      <c r="E10" s="487"/>
-      <c r="F10" s="488" t="s">
+      <c r="D10" s="495"/>
+      <c r="E10" s="495"/>
+      <c r="F10" s="496" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="488"/>
-      <c r="H10" s="488" t="s">
+      <c r="G10" s="496"/>
+      <c r="H10" s="496" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="488"/>
-      <c r="J10" s="489" t="s">
+      <c r="I10" s="496"/>
+      <c r="J10" s="497" t="s">
         <v>70</v>
       </c>
-      <c r="K10" s="489"/>
+      <c r="K10" s="497"/>
     </row>
     <row r="11" spans="1:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="20" t="s">
@@ -42959,25 +43037,25 @@
       <c r="I26" s="11"/>
     </row>
     <row r="27" spans="1:12" s="1" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="486" t="s">
+      <c r="C27" s="494" t="s">
         <v>81</v>
       </c>
-      <c r="D27" s="486"/>
-      <c r="E27" s="486"/>
-      <c r="F27" s="486"/>
+      <c r="D27" s="494"/>
+      <c r="E27" s="494"/>
+      <c r="F27" s="494"/>
       <c r="G27" s="67"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
     </row>
     <row r="28" spans="1:12" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="490" t="s">
+      <c r="C28" s="498" t="s">
         <v>82</v>
       </c>
-      <c r="D28" s="490"/>
-      <c r="E28" s="491" t="s">
+      <c r="D28" s="498"/>
+      <c r="E28" s="499" t="s">
         <v>83</v>
       </c>
-      <c r="F28" s="491"/>
+      <c r="F28" s="499"/>
       <c r="G28" s="67"/>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
@@ -42987,15 +43065,15 @@
         <v>84</v>
       </c>
       <c r="B29" s="69"/>
-      <c r="C29" s="492">
+      <c r="C29" s="500">
         <v>1</v>
       </c>
-      <c r="D29" s="492"/>
-      <c r="E29" s="493">
+      <c r="D29" s="500"/>
+      <c r="E29" s="501">
         <f>Data_day!B2</f>
         <v>0</v>
       </c>
-      <c r="F29" s="493"/>
+      <c r="F29" s="501"/>
       <c r="G29" s="67"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
@@ -43005,15 +43083,15 @@
         <v>85</v>
       </c>
       <c r="B30" s="71"/>
-      <c r="C30" s="494">
+      <c r="C30" s="502">
         <v>1</v>
       </c>
-      <c r="D30" s="494"/>
-      <c r="E30" s="495">
+      <c r="D30" s="502"/>
+      <c r="E30" s="503">
         <f>Data_day!C2</f>
         <v>0</v>
       </c>
-      <c r="F30" s="495"/>
+      <c r="F30" s="503"/>
       <c r="G30" s="67"/>
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
@@ -43023,15 +43101,15 @@
         <v>86</v>
       </c>
       <c r="B31" s="71"/>
-      <c r="C31" s="494">
+      <c r="C31" s="502">
         <v>1</v>
       </c>
-      <c r="D31" s="494"/>
-      <c r="E31" s="495">
+      <c r="D31" s="502"/>
+      <c r="E31" s="503">
         <f>Data_day!D2</f>
         <v>0</v>
       </c>
-      <c r="F31" s="495"/>
+      <c r="F31" s="503"/>
       <c r="G31" s="67"/>
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
@@ -43041,15 +43119,15 @@
         <v>87</v>
       </c>
       <c r="B32" s="71"/>
-      <c r="C32" s="494">
+      <c r="C32" s="502">
         <v>1</v>
       </c>
-      <c r="D32" s="494"/>
-      <c r="E32" s="495">
+      <c r="D32" s="502"/>
+      <c r="E32" s="503">
         <f>Data_day!E2</f>
         <v>0</v>
       </c>
-      <c r="F32" s="495"/>
+      <c r="F32" s="503"/>
       <c r="G32" s="67"/>
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
@@ -43059,15 +43137,15 @@
         <v>88</v>
       </c>
       <c r="B33" s="73"/>
-      <c r="C33" s="496">
+      <c r="C33" s="504">
         <v>1</v>
       </c>
-      <c r="D33" s="496"/>
-      <c r="E33" s="497">
+      <c r="D33" s="504"/>
+      <c r="E33" s="505">
         <f>Data_day!F2</f>
         <v>0</v>
       </c>
-      <c r="F33" s="497"/>
+      <c r="F33" s="505"/>
       <c r="G33" s="67"/>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
@@ -43088,15 +43166,15 @@
         <v>89</v>
       </c>
       <c r="B35" s="69"/>
-      <c r="C35" s="498">
+      <c r="C35" s="506">
         <v>1</v>
       </c>
-      <c r="D35" s="498"/>
-      <c r="E35" s="493">
+      <c r="D35" s="506"/>
+      <c r="E35" s="501">
         <f>Data_day!G2</f>
         <v>0</v>
       </c>
-      <c r="F35" s="493"/>
+      <c r="F35" s="501"/>
       <c r="G35" s="67"/>
       <c r="I35" s="76"/>
       <c r="J35" s="76"/>
@@ -43107,15 +43185,15 @@
         <v>90</v>
       </c>
       <c r="B36" s="73"/>
-      <c r="C36" s="499">
+      <c r="C36" s="507">
         <v>1</v>
       </c>
-      <c r="D36" s="499"/>
-      <c r="E36" s="497">
+      <c r="D36" s="507"/>
+      <c r="E36" s="505">
         <f>Data_day!H2</f>
         <v>0</v>
       </c>
-      <c r="F36" s="497"/>
+      <c r="F36" s="505"/>
       <c r="G36" s="67"/>
       <c r="H36" s="77" t="s">
         <v>91</v>
@@ -43170,40 +43248,40 @@
       <c r="J41" s="66"/>
     </row>
     <row r="42" spans="1:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C42" s="486" t="s">
+      <c r="C42" s="494" t="s">
         <v>92</v>
       </c>
-      <c r="D42" s="486"/>
-      <c r="E42" s="486"/>
-      <c r="F42" s="486"/>
-      <c r="G42" s="486"/>
-      <c r="H42" s="486"/>
-      <c r="I42" s="486"/>
-      <c r="J42" s="486"/>
-      <c r="K42" s="486"/>
+      <c r="D42" s="494"/>
+      <c r="E42" s="494"/>
+      <c r="F42" s="494"/>
+      <c r="G42" s="494"/>
+      <c r="H42" s="494"/>
+      <c r="I42" s="494"/>
+      <c r="J42" s="494"/>
+      <c r="K42" s="494"/>
     </row>
     <row r="43" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C43" s="500" t="str">
+      <c r="C43" s="508" t="str">
         <f>C10</f>
         <v>Tous Véhicules</v>
       </c>
-      <c r="D43" s="500"/>
-      <c r="E43" s="500"/>
-      <c r="F43" s="501" t="str">
+      <c r="D43" s="508"/>
+      <c r="E43" s="508"/>
+      <c r="F43" s="509" t="str">
         <f>F10</f>
         <v>Véhicules légers</v>
       </c>
-      <c r="G43" s="501"/>
-      <c r="H43" s="501" t="str">
+      <c r="G43" s="509"/>
+      <c r="H43" s="509" t="str">
         <f>H10</f>
         <v>Poids lourds</v>
       </c>
-      <c r="I43" s="501"/>
-      <c r="J43" s="489" t="str">
+      <c r="I43" s="509"/>
+      <c r="J43" s="497" t="str">
         <f t="shared" ref="J43:J49" si="5">J10</f>
         <v>% Poids lourds</v>
       </c>
-      <c r="K43" s="489"/>
+      <c r="K43" s="497"/>
     </row>
     <row r="44" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C44" s="20" t="str">
@@ -43834,27 +43912,27 @@
     <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="39"/>
       <c r="B9" s="39"/>
-      <c r="C9" s="502" t="str">
+      <c r="C9" s="510" t="str">
         <f>CV_H!C10</f>
         <v>Tous Véhicules</v>
       </c>
-      <c r="D9" s="502"/>
-      <c r="E9" s="502"/>
-      <c r="F9" s="503" t="str">
+      <c r="D9" s="510"/>
+      <c r="E9" s="510"/>
+      <c r="F9" s="511" t="str">
         <f>CV_H!F10</f>
         <v>Véhicules légers</v>
       </c>
-      <c r="G9" s="503"/>
-      <c r="H9" s="504" t="str">
+      <c r="G9" s="511"/>
+      <c r="H9" s="512" t="str">
         <f>CV_H!H10</f>
         <v>Poids lourds</v>
       </c>
-      <c r="I9" s="504"/>
-      <c r="J9" s="505" t="str">
+      <c r="I9" s="512"/>
+      <c r="J9" s="513" t="str">
         <f>CV_H!J10</f>
         <v>% Poids lourds</v>
       </c>
-      <c r="K9" s="505"/>
+      <c r="K9" s="513"/>
     </row>
     <row r="10" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="39"/>
@@ -43978,12 +44056,12 @@
     </row>
     <row r="32" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:20" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="506" t="s">
+      <c r="A33" s="514" t="s">
         <v>97</v>
       </c>
-      <c r="B33" s="506"/>
-      <c r="C33" s="506"/>
-      <c r="D33" s="506"/>
+      <c r="B33" s="514"/>
+      <c r="C33" s="514"/>
+      <c r="D33" s="514"/>
       <c r="E33" s="39"/>
     </row>
     <row r="34" spans="1:20" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -44180,12 +44258,12 @@
         <f>CV_C!I23</f>
         <v>0</v>
       </c>
-      <c r="F44" s="507" t="s">
-        <v>183</v>
-      </c>
-      <c r="G44" s="508"/>
-      <c r="H44" s="508"/>
-      <c r="I44" s="505"/>
+      <c r="F44" s="515" t="s">
+        <v>182</v>
+      </c>
+      <c r="G44" s="516"/>
+      <c r="H44" s="516"/>
+      <c r="I44" s="513"/>
       <c r="J44" s="278"/>
       <c r="K44" s="67"/>
       <c r="L44" s="278"/>
@@ -44208,13 +44286,13 @@
         <f>CV_C!I24</f>
         <v>0</v>
       </c>
-      <c r="F45" s="509"/>
-      <c r="G45" s="510"/>
+      <c r="F45" s="517"/>
+      <c r="G45" s="518"/>
       <c r="H45" s="385" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I45" s="386" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J45" s="278"/>
       <c r="K45" s="67"/>
@@ -44264,12 +44342,12 @@
         <f>CV_C!I26</f>
         <v>0</v>
       </c>
-      <c r="F47" s="509" t="s">
-        <v>184</v>
-      </c>
-      <c r="G47" s="510"/>
+      <c r="F47" s="517" t="s">
+        <v>183</v>
+      </c>
+      <c r="G47" s="518"/>
       <c r="H47" s="247" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I47" s="393"/>
       <c r="J47" s="278"/>
@@ -44294,10 +44372,10 @@
         <f>CV_C!I27</f>
         <v>0</v>
       </c>
-      <c r="F48" s="509" t="s">
-        <v>180</v>
-      </c>
-      <c r="G48" s="510"/>
+      <c r="F48" s="517" t="s">
+        <v>179</v>
+      </c>
+      <c r="G48" s="518"/>
       <c r="H48" s="136" t="e">
         <f>I48/(I48+I54)</f>
         <v>#DIV/0!</v>
@@ -44354,12 +44432,12 @@
         <f>CV_C!I29</f>
         <v>0</v>
       </c>
-      <c r="F50" s="509" t="s">
-        <v>185</v>
-      </c>
-      <c r="G50" s="510"/>
+      <c r="F50" s="517" t="s">
+        <v>184</v>
+      </c>
+      <c r="G50" s="518"/>
       <c r="H50" s="247" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I50" s="249"/>
       <c r="J50" s="278"/>
@@ -44384,10 +44462,10 @@
         <f>CV_C!I30</f>
         <v>0</v>
       </c>
-      <c r="F51" s="509" t="s">
-        <v>181</v>
-      </c>
-      <c r="G51" s="510"/>
+      <c r="F51" s="517" t="s">
+        <v>180</v>
+      </c>
+      <c r="G51" s="518"/>
       <c r="H51" s="136" t="e">
         <f>I51/(I51+I57)</f>
         <v>#DIV/0!</v>
@@ -44444,12 +44522,12 @@
         <f>CV_C!I32</f>
         <v>0</v>
       </c>
-      <c r="F53" s="509" t="s">
-        <v>186</v>
-      </c>
-      <c r="G53" s="510"/>
+      <c r="F53" s="517" t="s">
+        <v>185</v>
+      </c>
+      <c r="G53" s="518"/>
       <c r="H53" s="247" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I53" s="249"/>
       <c r="J53"/>
@@ -44471,10 +44549,10 @@
         <f>CV_C!I33</f>
         <v>0</v>
       </c>
-      <c r="F54" s="509" t="s">
-        <v>180</v>
-      </c>
-      <c r="G54" s="510"/>
+      <c r="F54" s="517" t="s">
+        <v>179</v>
+      </c>
+      <c r="G54" s="518"/>
       <c r="H54" s="136" t="e">
         <f>I54/(I54+I48)</f>
         <v>#DIV/0!</v>
@@ -44525,12 +44603,12 @@
         <f>CV_C!I35</f>
         <v>0</v>
       </c>
-      <c r="F56" s="509" t="s">
-        <v>187</v>
-      </c>
-      <c r="G56" s="511"/>
+      <c r="F56" s="517" t="s">
+        <v>186</v>
+      </c>
+      <c r="G56" s="519"/>
       <c r="H56" s="247" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I56" s="249"/>
       <c r="J56"/>
@@ -44552,10 +44630,10 @@
         <f>CV_C!I36</f>
         <v>0</v>
       </c>
-      <c r="F57" s="509" t="s">
-        <v>181</v>
-      </c>
-      <c r="G57" s="511"/>
+      <c r="F57" s="517" t="s">
+        <v>180</v>
+      </c>
+      <c r="G57" s="519"/>
       <c r="H57" s="136" t="e">
         <f>I57/(I57+I51)</f>
         <v>#DIV/0!</v>
@@ -44651,7 +44729,8 @@
     <col min="1" max="1" width="10" style="1" customWidth="1"/>
     <col min="2" max="10" width="7.28515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="1.42578125" style="1" customWidth="1"/>
-    <col min="12" max="20" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="18" width="7.140625" style="1" customWidth="1"/>
+    <col min="19" max="20" width="7.28515625" style="1" customWidth="1"/>
     <col min="21" max="21" width="1.42578125" style="1" customWidth="1"/>
     <col min="22" max="30" width="7.28515625" style="1" customWidth="1"/>
   </cols>
@@ -44755,41 +44834,41 @@
     <row r="11" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:30" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
-      <c r="B12" s="512" t="s">
+      <c r="B12" s="520" t="s">
         <v>104</v>
       </c>
-      <c r="C12" s="512"/>
-      <c r="D12" s="512"/>
-      <c r="E12" s="512"/>
-      <c r="F12" s="512"/>
-      <c r="G12" s="512"/>
-      <c r="H12" s="512"/>
-      <c r="I12" s="512"/>
-      <c r="J12" s="512"/>
+      <c r="C12" s="520"/>
+      <c r="D12" s="520"/>
+      <c r="E12" s="520"/>
+      <c r="F12" s="520"/>
+      <c r="G12" s="520"/>
+      <c r="H12" s="520"/>
+      <c r="I12" s="520"/>
+      <c r="J12" s="520"/>
       <c r="K12" s="154"/>
-      <c r="L12" s="512" t="s">
+      <c r="L12" s="520" t="s">
         <v>105</v>
       </c>
-      <c r="M12" s="512"/>
-      <c r="N12" s="512"/>
-      <c r="O12" s="512"/>
-      <c r="P12" s="512"/>
-      <c r="Q12" s="512"/>
-      <c r="R12" s="512"/>
-      <c r="S12" s="512"/>
-      <c r="T12" s="512"/>
+      <c r="M12" s="520"/>
+      <c r="N12" s="520"/>
+      <c r="O12" s="520"/>
+      <c r="P12" s="520"/>
+      <c r="Q12" s="520"/>
+      <c r="R12" s="520"/>
+      <c r="S12" s="520"/>
+      <c r="T12" s="520"/>
       <c r="U12" s="154"/>
-      <c r="V12" s="512" t="s">
+      <c r="V12" s="520" t="s">
         <v>106</v>
       </c>
-      <c r="W12" s="512"/>
-      <c r="X12" s="512"/>
-      <c r="Y12" s="512"/>
-      <c r="Z12" s="512"/>
-      <c r="AA12" s="512"/>
-      <c r="AB12" s="512"/>
-      <c r="AC12" s="512"/>
-      <c r="AD12" s="512"/>
+      <c r="W12" s="520"/>
+      <c r="X12" s="520"/>
+      <c r="Y12" s="520"/>
+      <c r="Z12" s="520"/>
+      <c r="AA12" s="520"/>
+      <c r="AB12" s="520"/>
+      <c r="AC12" s="520"/>
+      <c r="AD12" s="520"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="155" t="s">
@@ -47975,21 +48054,21 @@
       <c r="I10" s="67"/>
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="486" t="str">
+      <c r="B11" s="494" t="str">
         <f>"Distrubution des classes SWISS7 par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)"</f>
         <v>Distrubution des classes SWISS7 par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)</v>
       </c>
-      <c r="C11" s="486"/>
-      <c r="D11" s="486"/>
-      <c r="E11" s="486"/>
-      <c r="F11" s="486"/>
-      <c r="G11" s="486"/>
-      <c r="H11" s="486"/>
+      <c r="C11" s="494"/>
+      <c r="D11" s="494"/>
+      <c r="E11" s="494"/>
+      <c r="F11" s="494"/>
+      <c r="G11" s="494"/>
+      <c r="H11" s="494"/>
       <c r="I11" s="233"/>
       <c r="J11" s="234" t="s">
         <v>108</v>
       </c>
-      <c r="K11" s="513" t="s">
+      <c r="K11" s="521" t="s">
         <v>111</v>
       </c>
     </row>
@@ -48022,7 +48101,7 @@
       <c r="J12" s="238" t="s">
         <v>101</v>
       </c>
-      <c r="K12" s="513"/>
+      <c r="K12" s="521"/>
     </row>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="239" t="s">
@@ -49134,12 +49213,20 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="11"/>
-      <c r="C40" s="10" t="e">
+      <c r="B40" s="484" t="s">
+        <v>207</v>
+      </c>
+      <c r="C40" s="485" t="e">
         <f>SUM(C37:E37)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H40" s="10" t="e">
+      <c r="D40" s="486"/>
+      <c r="E40" s="486"/>
+      <c r="F40" s="486"/>
+      <c r="G40" s="487" t="s">
+        <v>206</v>
+      </c>
+      <c r="H40" s="485" t="e">
         <f>SUM(B37,F37:H37)</f>
         <v>#DIV/0!</v>
       </c>
@@ -49159,22 +49246,22 @@
     </row>
     <row r="43" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5"/>
-      <c r="B43" s="486" t="str">
+      <c r="B43" s="494" t="str">
         <f>B11</f>
         <v>Distrubution des classes SWISS7 par tranche horaire  -  Cumuls sur 7 jours (Lu - Di)</v>
       </c>
-      <c r="C43" s="486"/>
-      <c r="D43" s="486"/>
-      <c r="E43" s="486"/>
-      <c r="F43" s="486"/>
-      <c r="G43" s="486"/>
-      <c r="H43" s="486"/>
+      <c r="C43" s="494"/>
+      <c r="D43" s="494"/>
+      <c r="E43" s="494"/>
+      <c r="F43" s="494"/>
+      <c r="G43" s="494"/>
+      <c r="H43" s="494"/>
       <c r="I43" s="233"/>
       <c r="J43" s="234" t="str">
         <f>J11</f>
         <v>THM</v>
       </c>
-      <c r="K43" s="513" t="str">
+      <c r="K43" s="521" t="str">
         <f>K11</f>
         <v>Part du TJM</v>
       </c>
@@ -49215,7 +49302,7 @@
       <c r="J44" s="238" t="s">
         <v>101</v>
       </c>
-      <c r="K44" s="513"/>
+      <c r="K44" s="521"/>
     </row>
     <row r="45" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="239" t="s">
@@ -50327,11 +50414,20 @@
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C72" s="10" t="e">
+      <c r="B72" s="484" t="s">
+        <v>207</v>
+      </c>
+      <c r="C72" s="485" t="e">
         <f>SUM(C69:E69)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H72" s="10" t="e">
+      <c r="D72" s="486"/>
+      <c r="E72" s="486"/>
+      <c r="F72" s="486"/>
+      <c r="G72" s="487" t="s">
+        <v>206</v>
+      </c>
+      <c r="H72" s="485" t="e">
         <f>SUM(B69,F69:H69)</f>
         <v>#DIV/0!</v>
       </c>
@@ -50400,14 +50496,14 @@
       <c r="C76" s="279"/>
       <c r="D76" s="279"/>
       <c r="E76" s="279"/>
-      <c r="F76" s="514" t="s">
+      <c r="F76" s="522" t="s">
         <v>129</v>
       </c>
-      <c r="G76" s="514"/>
-      <c r="H76" s="514"/>
-      <c r="I76" s="514"/>
-      <c r="J76" s="514"/>
-      <c r="K76" s="514"/>
+      <c r="G76" s="522"/>
+      <c r="H76" s="522"/>
+      <c r="I76" s="522"/>
+      <c r="J76" s="522"/>
+      <c r="K76" s="522"/>
       <c r="L76" s="278"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
@@ -50429,10 +50525,10 @@
       <c r="D78" s="67"/>
       <c r="E78" s="67"/>
       <c r="F78" s="67"/>
-      <c r="G78" s="67" t="s">
+      <c r="G78" s="531" t="s">
         <v>164</v>
       </c>
-      <c r="H78" s="349" t="e">
+      <c r="H78" s="491" t="e">
         <f>SUM(B45:B68,B13:B36,F13:H36,F45:H68)/SUM(B45:H68,B13:H36)</f>
         <v>#DIV/0!</v>
       </c>
@@ -50633,17 +50729,17 @@
     </row>
     <row r="11" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I11" s="282"/>
-      <c r="J11" s="515" t="s">
+      <c r="J11" s="523" t="s">
         <v>98</v>
       </c>
-      <c r="K11" s="516" t="s">
+      <c r="K11" s="524" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I12" s="249"/>
-      <c r="J12" s="515"/>
-      <c r="K12" s="516"/>
+      <c r="J12" s="523"/>
+      <c r="K12" s="524"/>
     </row>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I13" s="249"/>
@@ -51049,18 +51145,18 @@
     <row r="45" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I46" s="302"/>
-      <c r="J46" s="515" t="s">
+      <c r="J46" s="523" t="s">
         <v>98</v>
       </c>
-      <c r="K46" s="516" t="str">
+      <c r="K46" s="524" t="str">
         <f>K11</f>
         <v>Part du TJM</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I47" s="303"/>
-      <c r="J47" s="515"/>
-      <c r="K47" s="516"/>
+      <c r="J47" s="523"/>
+      <c r="K47" s="524"/>
     </row>
     <row r="48" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I48" s="303"/>

</xml_diff>